<commit_message>
FINAL- Olga, Blanca, incorporate Kevin, Andrew, Diamond
</commit_message>
<xml_diff>
--- a/Resources/NBA_TeamMarketSize_orig.xlsx
+++ b/Resources/NBA_TeamMarketSize_orig.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{D225EC82-AD9A-412D-BFD1-448256B2736E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{A4E647AE-0FA7-4EA4-B829-9A85C0B1648C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -106,9 +106,6 @@
     <t>Los Angeles Lakers</t>
   </si>
   <si>
-    <t>Brookyn Nets</t>
-  </si>
-  <si>
     <t>New York Knicks</t>
   </si>
   <si>
@@ -128,6 +125,9 @@
   </si>
   <si>
     <t>Small</t>
+  </si>
+  <si>
+    <t>Brooklyn Nets</t>
   </si>
 </sst>
 </file>
@@ -511,8 +511,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C31" sqref="C22:C31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -524,13 +524,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>31</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -538,10 +538,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -549,10 +549,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="C3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -563,7 +563,7 @@
         <v>27</v>
       </c>
       <c r="C4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -574,7 +574,7 @@
         <v>26</v>
       </c>
       <c r="C5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -585,7 +585,7 @@
         <v>0</v>
       </c>
       <c r="C6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -596,7 +596,7 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -607,7 +607,7 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -618,7 +618,7 @@
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -629,7 +629,7 @@
         <v>4</v>
       </c>
       <c r="C10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -640,7 +640,7 @@
         <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -651,7 +651,7 @@
         <v>6</v>
       </c>
       <c r="C12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -662,7 +662,7 @@
         <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -673,7 +673,7 @@
         <v>8</v>
       </c>
       <c r="C14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -684,7 +684,7 @@
         <v>9</v>
       </c>
       <c r="C15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -695,7 +695,7 @@
         <v>10</v>
       </c>
       <c r="C16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -706,7 +706,7 @@
         <v>11</v>
       </c>
       <c r="C17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -717,7 +717,7 @@
         <v>12</v>
       </c>
       <c r="C18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -728,7 +728,7 @@
         <v>13</v>
       </c>
       <c r="C19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -739,7 +739,7 @@
         <v>14</v>
       </c>
       <c r="C20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -750,7 +750,7 @@
         <v>15</v>
       </c>
       <c r="C21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -761,7 +761,7 @@
         <v>16</v>
       </c>
       <c r="C22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -772,7 +772,7 @@
         <v>17</v>
       </c>
       <c r="C23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -783,7 +783,7 @@
         <v>18</v>
       </c>
       <c r="C24" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -794,7 +794,7 @@
         <v>19</v>
       </c>
       <c r="C25" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -805,7 +805,7 @@
         <v>20</v>
       </c>
       <c r="C26" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -816,7 +816,7 @@
         <v>21</v>
       </c>
       <c r="C27" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -827,7 +827,7 @@
         <v>22</v>
       </c>
       <c r="C28" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -838,7 +838,7 @@
         <v>23</v>
       </c>
       <c r="C29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -849,7 +849,7 @@
         <v>24</v>
       </c>
       <c r="C30" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -860,7 +860,7 @@
         <v>25</v>
       </c>
       <c r="C31" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>